<commit_message>
[PHOENIX-6394] updated demolition of property
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,641 +26,682 @@
     <sheet name="searchDetails" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="revisionPetitionDetails" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="hearingDetails" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="demolitionDetails" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="208">
-  <si>
-    <t xml:space="preserve">dataName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobileNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ownerName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emailAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">guardianRelation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">guardian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bimal@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Father</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasonForCreation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extentOfSite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupancyCertificateNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentNewProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW PROPERTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zoneNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wardNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blockNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electionWard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pincode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addressOne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4th colony</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Election Ward No. 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toilets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterTap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attachedBathroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterHarvesting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cableConnection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">floorType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roofType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wallType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">woodType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">defaultConstructionType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAMBOO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allmixing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">floorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">classificationOfBuilding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">natureOfUsage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firmName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupantName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constructionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">effectiveFromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unstructuredLand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">breadth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buildingPermissionNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buildingPermissionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstFloor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st floor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deedNo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deedDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentSelect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registered Will Document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approverDepartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approverDesignation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approverRemarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">billCollector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REVENUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bill Collector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D.Khasim ~ REV_Bill Collector_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to bill collector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenueInspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UD Revenue Inspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P.Sadiq Hussain ~ UD RI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to revenue insoector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenueOfficer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revenue Officer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B.Veeraswamy ~ REV_Revenue Officer_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to revenue officer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADMINISTRATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ravindra Babu ~ ADM_Commissioner_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commissioner1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ravindra Babu/ADM_Commissioner_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENGINEERING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assistant Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C.Naresh/ENG_Assistant Engineer_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">engineer1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACCOUNTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assistant Examiner of Accounts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hanuman Prasad ~ ACC_AEOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer1a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K.Mohammed Juneed ~ ACC_AEOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Examiner of Accounts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D Ramachandra Reddy ~ ACC_EOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D Ramachandra Reddy/ACC_EOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deputyExecutiveEngineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deputy Executive Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sanitaryInspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUBLIC HEALTH AND SANITATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sanitary Inspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chandragiri Murali Krishna ~ PHS_Sanitary Inspector_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to Sanitary Inspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">propertyType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categoryOfOwnership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">residentialPrivate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Private</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentAdditionProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editfloorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editclassificationOfBuilding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editnatureOfUsage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editfirmName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editoccupancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editoccupantName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editconstructionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editeffectiveFromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editunstructuredLand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editlength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbreadth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbuildingPermissionNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbuildingPermissionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editplinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstFloorAdditionaltaration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd Floor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commercial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">report1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">report2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">message1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">actualMessage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">message</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sellerExecutantName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buyerClaimantName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doorNo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">propertyAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registeredPlotArea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registerPlinthArea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eastBoundary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">westBoundary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">northBoundary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">southBoundary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sroName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasonForChange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registrationDocumentNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registrationDocumentDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">partiesConsiderationValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">departmentGuide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nadir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bangalore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gift Deed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataRow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchValue2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchWithAssessmentNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchWithMobileNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000161311</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchWithDoorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87/1110-9-c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchWithZoneAndWardNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone-15;Revenue Ward No  87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87/1110-9-c;C. Naga Sailaja W/o R. Satish Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchWithOwnerName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenue colony;C. Naga Sailaja W/o R. Satish Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchByDemand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">500;501</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revisionPetitionDetails</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revisionpetitionBlock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revision Started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hearingDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hearingTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">venue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hearingBlock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28/06/2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.30 AM</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="223">
+  <si>
+    <t>dataName</t>
+  </si>
+  <si>
+    <t>mobileNumber</t>
+  </si>
+  <si>
+    <t>ownerName</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>emailAddress</t>
+  </si>
+  <si>
+    <t>guardianRelation</t>
+  </si>
+  <si>
+    <t>guardian</t>
+  </si>
+  <si>
+    <t>bimal</t>
+  </si>
+  <si>
+    <t>Bimal</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>bimal@gmail.com</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>reasonForCreation</t>
+  </si>
+  <si>
+    <t>extentOfSite</t>
+  </si>
+  <si>
+    <t>occupancyCertificateNumber</t>
+  </si>
+  <si>
+    <t>assessmentNewProperty</t>
+  </si>
+  <si>
+    <t>NEW PROPERTY</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>zoneNumber</t>
+  </si>
+  <si>
+    <t>wardNumber</t>
+  </si>
+  <si>
+    <t>blockNumber</t>
+  </si>
+  <si>
+    <t>electionWard</t>
+  </si>
+  <si>
+    <t>doorNumber</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>addressOne</t>
+  </si>
+  <si>
+    <t>4th colony</t>
+  </si>
+  <si>
+    <t>Zone-1</t>
+  </si>
+  <si>
+    <t>Election Ward No. 1</t>
+  </si>
+  <si>
+    <t>12/46</t>
+  </si>
+  <si>
+    <t>lift</t>
+  </si>
+  <si>
+    <t>toilets</t>
+  </si>
+  <si>
+    <t>waterTap</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>attachedBathroom</t>
+  </si>
+  <si>
+    <t>waterHarvesting</t>
+  </si>
+  <si>
+    <t>cableConnection</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>floorType</t>
+  </si>
+  <si>
+    <t>roofType</t>
+  </si>
+  <si>
+    <t>wallType</t>
+  </si>
+  <si>
+    <t>woodType</t>
+  </si>
+  <si>
+    <t>defaultConstructionType</t>
+  </si>
+  <si>
+    <t>BAMBOO</t>
+  </si>
+  <si>
+    <t>Absheet</t>
+  </si>
+  <si>
+    <t>Allmixing</t>
+  </si>
+  <si>
+    <t>floorNumber</t>
+  </si>
+  <si>
+    <t>classificationOfBuilding</t>
+  </si>
+  <si>
+    <t>natureOfUsage</t>
+  </si>
+  <si>
+    <t>firmName</t>
+  </si>
+  <si>
+    <t>occupancy</t>
+  </si>
+  <si>
+    <t>occupantName</t>
+  </si>
+  <si>
+    <t>constructionDate</t>
+  </si>
+  <si>
+    <t>effectiveFromDate</t>
+  </si>
+  <si>
+    <t>unstructuredLand</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>breadth</t>
+  </si>
+  <si>
+    <t>buildingPermissionNumber</t>
+  </si>
+  <si>
+    <t>buildingPermissionDate</t>
+  </si>
+  <si>
+    <t>plinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t>firstFloor</t>
+  </si>
+  <si>
+    <t>1st floor</t>
+  </si>
+  <si>
+    <t>Huts</t>
+  </si>
+  <si>
+    <t>Residence</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>11/22</t>
+  </si>
+  <si>
+    <t>documentType</t>
+  </si>
+  <si>
+    <t>deedNo</t>
+  </si>
+  <si>
+    <t>deedDate</t>
+  </si>
+  <si>
+    <t>documentSelect</t>
+  </si>
+  <si>
+    <t>Registered Will Document</t>
+  </si>
+  <si>
+    <t>43051</t>
+  </si>
+  <si>
+    <t>20/12/2016</t>
+  </si>
+  <si>
+    <t>approverDepartment</t>
+  </si>
+  <si>
+    <t>approverDesignation</t>
+  </si>
+  <si>
+    <t>approver</t>
+  </si>
+  <si>
+    <t>approverRemarks</t>
+  </si>
+  <si>
+    <t>billCollector</t>
+  </si>
+  <si>
+    <t>REVENUE</t>
+  </si>
+  <si>
+    <t>Bill Collector</t>
+  </si>
+  <si>
+    <t>D.Khasim ~ REV_Bill Collector_1</t>
+  </si>
+  <si>
+    <t>Forward to bill collector</t>
+  </si>
+  <si>
+    <t>revenueInspector</t>
+  </si>
+  <si>
+    <t>UD Revenue Inspector</t>
+  </si>
+  <si>
+    <t>P.Sadiq Hussain ~ UD RI</t>
+  </si>
+  <si>
+    <t>Forward to revenue insoector</t>
+  </si>
+  <si>
+    <t>revenueOfficer</t>
+  </si>
+  <si>
+    <t>Revenue Officer</t>
+  </si>
+  <si>
+    <t>B.Veeraswamy ~ REV_Revenue Officer_3</t>
+  </si>
+  <si>
+    <t>Forward to revenue officer</t>
+  </si>
+  <si>
+    <t>commissioner</t>
+  </si>
+  <si>
+    <t>ADMINISTRATION</t>
+  </si>
+  <si>
+    <t>Commissioner</t>
+  </si>
+  <si>
+    <t>Ravindra Babu ~ ADM_Commissioner_2</t>
+  </si>
+  <si>
+    <t>Forward to commissioner</t>
+  </si>
+  <si>
+    <t>commissioner1</t>
+  </si>
+  <si>
+    <t>Ravindra Babu/ADM_Commissioner_2</t>
+  </si>
+  <si>
+    <t>engineer</t>
+  </si>
+  <si>
+    <t>ENGINEERING</t>
+  </si>
+  <si>
+    <t>Assistant Engineer</t>
+  </si>
+  <si>
+    <t>C.Naresh/ENG_Assistant Engineer_4</t>
+  </si>
+  <si>
+    <t>Forward to Engineer</t>
+  </si>
+  <si>
+    <t>engineer1</t>
+  </si>
+  <si>
+    <t>A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
+  </si>
+  <si>
+    <t>accountOfficer1</t>
+  </si>
+  <si>
+    <t>ACCOUNTS</t>
+  </si>
+  <si>
+    <t>Assistant Examiner of Accounts</t>
+  </si>
+  <si>
+    <t>Hanuman Prasad ~ ACC_AEOA_1</t>
+  </si>
+  <si>
+    <t>accountOfficer1a</t>
+  </si>
+  <si>
+    <t>K.Mohammed Juneed ~ ACC_AEOA_1</t>
+  </si>
+  <si>
+    <t>accountOfficer2</t>
+  </si>
+  <si>
+    <t>Examiner of Accounts</t>
+  </si>
+  <si>
+    <t>D Ramachandra Reddy ~ ACC_EOA_1</t>
+  </si>
+  <si>
+    <t>accountOfficer3</t>
+  </si>
+  <si>
+    <t>D Ramachandra Reddy/ACC_EOA_1</t>
+  </si>
+  <si>
+    <t>deputyExecutiveEngineer</t>
+  </si>
+  <si>
+    <t>Deputy Executive Engineer</t>
+  </si>
+  <si>
+    <t>S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
+  </si>
+  <si>
+    <t>sanitaryInspector</t>
+  </si>
+  <si>
+    <t>PUBLIC HEALTH AND SANITATION</t>
+  </si>
+  <si>
+    <t>Sanitary Inspector</t>
+  </si>
+  <si>
+    <t>Chandragiri Murali Krishna ~ PHS_Sanitary Inspector_1</t>
+  </si>
+  <si>
+    <t>Forward to Sanitary Inspector</t>
+  </si>
+  <si>
+    <t>propertyType</t>
+  </si>
+  <si>
+    <t>categoryOfOwnership</t>
+  </si>
+  <si>
+    <t>residentialPrivate</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>assessmentAdditionProperty</t>
+  </si>
+  <si>
+    <t>editfloorNumber</t>
+  </si>
+  <si>
+    <t>editclassificationOfBuilding</t>
+  </si>
+  <si>
+    <t>editnatureOfUsage</t>
+  </si>
+  <si>
+    <t>editfirmName</t>
+  </si>
+  <si>
+    <t>editoccupancy</t>
+  </si>
+  <si>
+    <t>editoccupantName</t>
+  </si>
+  <si>
+    <t>editconstructionDate</t>
+  </si>
+  <si>
+    <t>editeffectiveFromDate</t>
+  </si>
+  <si>
+    <t>editunstructuredLand</t>
+  </si>
+  <si>
+    <t>editlength</t>
+  </si>
+  <si>
+    <t>editbreadth</t>
+  </si>
+  <si>
+    <t>editbuildingPermissionNumber</t>
+  </si>
+  <si>
+    <t>editbuildingPermissionDate</t>
+  </si>
+  <si>
+    <t>editplinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t>firstFloorAdditionaltaration</t>
+  </si>
+  <si>
+    <t>2nd Floor</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>Sunil</t>
+  </si>
+  <si>
+    <t>33/22</t>
+  </si>
+  <si>
+    <t>fromDate</t>
+  </si>
+  <si>
+    <t>toDate</t>
+  </si>
+  <si>
+    <t>report1</t>
+  </si>
+  <si>
+    <t>06/12/2016</t>
+  </si>
+  <si>
+    <t>report2</t>
+  </si>
+  <si>
+    <t>07/12/2016</t>
+  </si>
+  <si>
+    <t>10/12/2016</t>
+  </si>
+  <si>
+    <t>message1</t>
+  </si>
+  <si>
+    <t>actualMessage</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>sellerExecutantName</t>
+  </si>
+  <si>
+    <t>buyerClaimantName</t>
+  </si>
+  <si>
+    <t>doorNo</t>
+  </si>
+  <si>
+    <t>propertyAddress</t>
+  </si>
+  <si>
+    <t>registeredPlotArea</t>
+  </si>
+  <si>
+    <t>registerPlinthArea</t>
+  </si>
+  <si>
+    <t>eastBoundary</t>
+  </si>
+  <si>
+    <t>westBoundary</t>
+  </si>
+  <si>
+    <t>northBoundary</t>
+  </si>
+  <si>
+    <t>southBoundary</t>
+  </si>
+  <si>
+    <t>sroName</t>
+  </si>
+  <si>
+    <t>reasonForChange</t>
+  </si>
+  <si>
+    <t>registrationDocumentNumber</t>
+  </si>
+  <si>
+    <t>registrationDocumentDate</t>
+  </si>
+  <si>
+    <t>partiesConsiderationValue</t>
+  </si>
+  <si>
+    <t>departmentGuide</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>Nadir</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Sro</t>
+  </si>
+  <si>
+    <t>Gift Deed</t>
+  </si>
+  <si>
+    <t>12/12/2016</t>
+  </si>
+  <si>
+    <t>dataRow</t>
+  </si>
+  <si>
+    <t>searchValue</t>
+  </si>
+  <si>
+    <t>searchValue2</t>
+  </si>
+  <si>
+    <t>searchWithAssessmentNumber</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>searchWithMobileNumber</t>
+  </si>
+  <si>
+    <t>0000161311</t>
+  </si>
+  <si>
+    <t>searchWithDoorNumber</t>
+  </si>
+  <si>
+    <t>87/1110-9-c</t>
+  </si>
+  <si>
+    <t>searchWithZoneAndWardNumber</t>
+  </si>
+  <si>
+    <t>Zone-15;Revenue Ward No  87</t>
+  </si>
+  <si>
+    <t>87/1110-9-c;C. Naga Sailaja W/o R. Satish Kumar</t>
+  </si>
+  <si>
+    <t>searchWithOwnerName</t>
+  </si>
+  <si>
+    <t>revenue colony;C. Naga Sailaja W/o R. Satish Kumar</t>
+  </si>
+  <si>
+    <t>searchByDemand</t>
+  </si>
+  <si>
+    <t>500;501</t>
+  </si>
+  <si>
+    <t>revisionPetitionDetails</t>
+  </si>
+  <si>
+    <t>revisionpetitionBlock</t>
+  </si>
+  <si>
+    <t>Revision Started</t>
+  </si>
+  <si>
+    <t>hearingDate</t>
+  </si>
+  <si>
+    <t>hearingTime</t>
+  </si>
+  <si>
+    <t>venue</t>
+  </si>
+  <si>
+    <t>hearingBlock</t>
+  </si>
+  <si>
+    <t>28/06/2017</t>
+  </si>
+  <si>
+    <t>9.30 AM</t>
+  </si>
+  <si>
+    <t>reasonForDemolition</t>
+  </si>
+  <si>
+    <t>surveyNumber</t>
+  </si>
+  <si>
+    <t>pattaNumber</t>
+  </si>
+  <si>
+    <t>marketValue</t>
+  </si>
+  <si>
+    <t>capitalValue</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>demolitionBlock</t>
+  </si>
+  <si>
+    <t>Demolition of property</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>pqr</t>
+  </si>
+  <si>
+    <t>lmn</t>
   </si>
 </sst>
 </file>
@@ -668,7 +709,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
@@ -899,6 +940,7 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.44897959183673"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="1" width="27.8061224489796"/>
     <col collapsed="false" hidden="false" max="257" min="7" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,7 +995,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1006,7 +1048,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1135,7 +1177,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1150,7 +1192,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1160,6 +1202,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.9744897959184"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.3775510204082"/>
     <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1187,7 +1230,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1240,7 +1283,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1286,7 +1329,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1325,6 +1368,7 @@
     <col collapsed="false" hidden="false" max="16" min="16" style="1" width="21.1938775510204"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="1" width="24.5663265306122"/>
     <col collapsed="false" hidden="false" max="257" min="18" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1436,7 +1480,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1539,7 +1583,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1584,7 +1628,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1600,7 +1644,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1639,7 +1683,98 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1666,6 +1801,7 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="48.3265306122449"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.7448979591837"/>
     <col collapsed="false" hidden="false" max="256" min="6" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1701,7 +1837,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1729,6 +1865,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="32.3979591836735"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.0612244897959"/>
     <col collapsed="false" hidden="false" max="257" min="8" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,7 +1917,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1802,6 +1939,7 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="257" min="1" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1866,7 +2004,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1889,6 +2027,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40.5"/>
     <col collapsed="false" hidden="false" max="257" min="2" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,7 +2069,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1969,6 +2108,7 @@
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.44897959183673"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.9030612244898"/>
     <col collapsed="false" hidden="false" max="257" min="19" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2068,7 +2208,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2127,7 +2267,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2154,6 +2294,7 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="67.6326530612245"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="44.4132653061225"/>
     <col collapsed="false" hidden="false" max="257" min="6" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2403,7 +2544,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2428,6 +2569,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.1377551020408"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.1785714285714"/>
     <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2455,7 +2597,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[PHOENIX-6395] completed bifurcation of property
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,13 +27,14 @@
     <sheet name="revisionPetitionDetails" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="hearingDetails" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="demolitionDetails" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="bifurcationDetails" sheetId="20" state="visible" r:id="rId21"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="226">
   <si>
     <t>dataName</t>
   </si>
@@ -702,6 +703,15 @@
   </si>
   <si>
     <t>lmn</t>
+  </si>
+  <si>
+    <t>parentAssessmentNo</t>
+  </si>
+  <si>
+    <t>bifurcationProperty</t>
+  </si>
+  <si>
+    <t>BIFURCATION</t>
   </si>
 </sst>
 </file>
@@ -1008,10 +1018,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1045,6 +1055,7 @@
         <v>111</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1063,7 +1074,7 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1296,10 +1307,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1326,6 +1337,7 @@
         <v>159</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1342,7 +1354,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
@@ -1477,6 +1489,7 @@
         <v>900000</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1570,7 +1583,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>197</v>
       </c>
@@ -1644,12 +1657,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1698,7 +1715,7 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1789,8 +1806,8 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1841,6 +1858,575 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:IW2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.7857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.5663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
+      <c r="AW1" s="1"/>
+      <c r="AX1" s="1"/>
+      <c r="AY1" s="1"/>
+      <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
+      <c r="BB1" s="1"/>
+      <c r="BC1" s="1"/>
+      <c r="BD1" s="1"/>
+      <c r="BE1" s="1"/>
+      <c r="BF1" s="1"/>
+      <c r="BG1" s="1"/>
+      <c r="BH1" s="1"/>
+      <c r="BI1" s="1"/>
+      <c r="BJ1" s="1"/>
+      <c r="BK1" s="1"/>
+      <c r="BL1" s="1"/>
+      <c r="BM1" s="1"/>
+      <c r="BN1" s="1"/>
+      <c r="BO1" s="1"/>
+      <c r="BP1" s="1"/>
+      <c r="BQ1" s="1"/>
+      <c r="BR1" s="1"/>
+      <c r="BS1" s="1"/>
+      <c r="BT1" s="1"/>
+      <c r="BU1" s="1"/>
+      <c r="BV1" s="1"/>
+      <c r="BW1" s="1"/>
+      <c r="BX1" s="1"/>
+      <c r="BY1" s="1"/>
+      <c r="BZ1" s="1"/>
+      <c r="CA1" s="1"/>
+      <c r="CB1" s="1"/>
+      <c r="CC1" s="1"/>
+      <c r="CD1" s="1"/>
+      <c r="CE1" s="1"/>
+      <c r="CF1" s="1"/>
+      <c r="CG1" s="1"/>
+      <c r="CH1" s="1"/>
+      <c r="CI1" s="1"/>
+      <c r="CJ1" s="1"/>
+      <c r="CK1" s="1"/>
+      <c r="CL1" s="1"/>
+      <c r="CM1" s="1"/>
+      <c r="CN1" s="1"/>
+      <c r="CO1" s="1"/>
+      <c r="CP1" s="1"/>
+      <c r="CQ1" s="1"/>
+      <c r="CR1" s="1"/>
+      <c r="CS1" s="1"/>
+      <c r="CT1" s="1"/>
+      <c r="CU1" s="1"/>
+      <c r="CV1" s="1"/>
+      <c r="CW1" s="1"/>
+      <c r="CX1" s="1"/>
+      <c r="CY1" s="1"/>
+      <c r="CZ1" s="1"/>
+      <c r="DA1" s="1"/>
+      <c r="DB1" s="1"/>
+      <c r="DC1" s="1"/>
+      <c r="DD1" s="1"/>
+      <c r="DE1" s="1"/>
+      <c r="DF1" s="1"/>
+      <c r="DG1" s="1"/>
+      <c r="DH1" s="1"/>
+      <c r="DI1" s="1"/>
+      <c r="DJ1" s="1"/>
+      <c r="DK1" s="1"/>
+      <c r="DL1" s="1"/>
+      <c r="DM1" s="1"/>
+      <c r="DN1" s="1"/>
+      <c r="DO1" s="1"/>
+      <c r="DP1" s="1"/>
+      <c r="DQ1" s="1"/>
+      <c r="DR1" s="1"/>
+      <c r="DS1" s="1"/>
+      <c r="DT1" s="1"/>
+      <c r="DU1" s="1"/>
+      <c r="DV1" s="1"/>
+      <c r="DW1" s="1"/>
+      <c r="DX1" s="1"/>
+      <c r="DY1" s="1"/>
+      <c r="DZ1" s="1"/>
+      <c r="EA1" s="1"/>
+      <c r="EB1" s="1"/>
+      <c r="EC1" s="1"/>
+      <c r="ED1" s="1"/>
+      <c r="EE1" s="1"/>
+      <c r="EF1" s="1"/>
+      <c r="EG1" s="1"/>
+      <c r="EH1" s="1"/>
+      <c r="EI1" s="1"/>
+      <c r="EJ1" s="1"/>
+      <c r="EK1" s="1"/>
+      <c r="EL1" s="1"/>
+      <c r="EM1" s="1"/>
+      <c r="EN1" s="1"/>
+      <c r="EO1" s="1"/>
+      <c r="EP1" s="1"/>
+      <c r="EQ1" s="1"/>
+      <c r="ER1" s="1"/>
+      <c r="ES1" s="1"/>
+      <c r="ET1" s="1"/>
+      <c r="EU1" s="1"/>
+      <c r="EV1" s="1"/>
+      <c r="EW1" s="1"/>
+      <c r="EX1" s="1"/>
+      <c r="EY1" s="1"/>
+      <c r="EZ1" s="1"/>
+      <c r="FA1" s="1"/>
+      <c r="FB1" s="1"/>
+      <c r="FC1" s="1"/>
+      <c r="FD1" s="1"/>
+      <c r="FE1" s="1"/>
+      <c r="FF1" s="1"/>
+      <c r="FG1" s="1"/>
+      <c r="FH1" s="1"/>
+      <c r="FI1" s="1"/>
+      <c r="FJ1" s="1"/>
+      <c r="FK1" s="1"/>
+      <c r="FL1" s="1"/>
+      <c r="FM1" s="1"/>
+      <c r="FN1" s="1"/>
+      <c r="FO1" s="1"/>
+      <c r="FP1" s="1"/>
+      <c r="FQ1" s="1"/>
+      <c r="FR1" s="1"/>
+      <c r="FS1" s="1"/>
+      <c r="FT1" s="1"/>
+      <c r="FU1" s="1"/>
+      <c r="FV1" s="1"/>
+      <c r="FW1" s="1"/>
+      <c r="FX1" s="1"/>
+      <c r="FY1" s="1"/>
+      <c r="FZ1" s="1"/>
+      <c r="GA1" s="1"/>
+      <c r="GB1" s="1"/>
+      <c r="GC1" s="1"/>
+      <c r="GD1" s="1"/>
+      <c r="GE1" s="1"/>
+      <c r="GF1" s="1"/>
+      <c r="GG1" s="1"/>
+      <c r="GH1" s="1"/>
+      <c r="GI1" s="1"/>
+      <c r="GJ1" s="1"/>
+      <c r="GK1" s="1"/>
+      <c r="GL1" s="1"/>
+      <c r="GM1" s="1"/>
+      <c r="GN1" s="1"/>
+      <c r="GO1" s="1"/>
+      <c r="GP1" s="1"/>
+      <c r="GQ1" s="1"/>
+      <c r="GR1" s="1"/>
+      <c r="GS1" s="1"/>
+      <c r="GT1" s="1"/>
+      <c r="GU1" s="1"/>
+      <c r="GV1" s="1"/>
+      <c r="GW1" s="1"/>
+      <c r="GX1" s="1"/>
+      <c r="GY1" s="1"/>
+      <c r="GZ1" s="1"/>
+      <c r="HA1" s="1"/>
+      <c r="HB1" s="1"/>
+      <c r="HC1" s="1"/>
+      <c r="HD1" s="1"/>
+      <c r="HE1" s="1"/>
+      <c r="HF1" s="1"/>
+      <c r="HG1" s="1"/>
+      <c r="HH1" s="1"/>
+      <c r="HI1" s="1"/>
+      <c r="HJ1" s="1"/>
+      <c r="HK1" s="1"/>
+      <c r="HL1" s="1"/>
+      <c r="HM1" s="1"/>
+      <c r="HN1" s="1"/>
+      <c r="HO1" s="1"/>
+      <c r="HP1" s="1"/>
+      <c r="HQ1" s="1"/>
+      <c r="HR1" s="1"/>
+      <c r="HS1" s="1"/>
+      <c r="HT1" s="1"/>
+      <c r="HU1" s="1"/>
+      <c r="HV1" s="1"/>
+      <c r="HW1" s="1"/>
+      <c r="HX1" s="1"/>
+      <c r="HY1" s="1"/>
+      <c r="HZ1" s="1"/>
+      <c r="IA1" s="1"/>
+      <c r="IB1" s="1"/>
+      <c r="IC1" s="1"/>
+      <c r="ID1" s="1"/>
+      <c r="IE1" s="1"/>
+      <c r="IF1" s="1"/>
+      <c r="IG1" s="1"/>
+      <c r="IH1" s="1"/>
+      <c r="II1" s="1"/>
+      <c r="IJ1" s="1"/>
+      <c r="IK1" s="1"/>
+      <c r="IL1" s="1"/>
+      <c r="IM1" s="1"/>
+      <c r="IN1" s="1"/>
+      <c r="IO1" s="1"/>
+      <c r="IP1" s="1"/>
+      <c r="IQ1" s="1"/>
+      <c r="IR1" s="1"/>
+      <c r="IS1" s="1"/>
+      <c r="IT1" s="1"/>
+      <c r="IU1" s="1"/>
+      <c r="IV1" s="1"/>
+      <c r="IW1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1016094473</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="1"/>
+      <c r="BC2" s="1"/>
+      <c r="BD2" s="1"/>
+      <c r="BE2" s="1"/>
+      <c r="BF2" s="1"/>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1"/>
+      <c r="BI2" s="1"/>
+      <c r="BJ2" s="1"/>
+      <c r="BK2" s="1"/>
+      <c r="BL2" s="1"/>
+      <c r="BM2" s="1"/>
+      <c r="BN2" s="1"/>
+      <c r="BO2" s="1"/>
+      <c r="BP2" s="1"/>
+      <c r="BQ2" s="1"/>
+      <c r="BR2" s="1"/>
+      <c r="BS2" s="1"/>
+      <c r="BT2" s="1"/>
+      <c r="BU2" s="1"/>
+      <c r="BV2" s="1"/>
+      <c r="BW2" s="1"/>
+      <c r="BX2" s="1"/>
+      <c r="BY2" s="1"/>
+      <c r="BZ2" s="1"/>
+      <c r="CA2" s="1"/>
+      <c r="CB2" s="1"/>
+      <c r="CC2" s="1"/>
+      <c r="CD2" s="1"/>
+      <c r="CE2" s="1"/>
+      <c r="CF2" s="1"/>
+      <c r="CG2" s="1"/>
+      <c r="CH2" s="1"/>
+      <c r="CI2" s="1"/>
+      <c r="CJ2" s="1"/>
+      <c r="CK2" s="1"/>
+      <c r="CL2" s="1"/>
+      <c r="CM2" s="1"/>
+      <c r="CN2" s="1"/>
+      <c r="CO2" s="1"/>
+      <c r="CP2" s="1"/>
+      <c r="CQ2" s="1"/>
+      <c r="CR2" s="1"/>
+      <c r="CS2" s="1"/>
+      <c r="CT2" s="1"/>
+      <c r="CU2" s="1"/>
+      <c r="CV2" s="1"/>
+      <c r="CW2" s="1"/>
+      <c r="CX2" s="1"/>
+      <c r="CY2" s="1"/>
+      <c r="CZ2" s="1"/>
+      <c r="DA2" s="1"/>
+      <c r="DB2" s="1"/>
+      <c r="DC2" s="1"/>
+      <c r="DD2" s="1"/>
+      <c r="DE2" s="1"/>
+      <c r="DF2" s="1"/>
+      <c r="DG2" s="1"/>
+      <c r="DH2" s="1"/>
+      <c r="DI2" s="1"/>
+      <c r="DJ2" s="1"/>
+      <c r="DK2" s="1"/>
+      <c r="DL2" s="1"/>
+      <c r="DM2" s="1"/>
+      <c r="DN2" s="1"/>
+      <c r="DO2" s="1"/>
+      <c r="DP2" s="1"/>
+      <c r="DQ2" s="1"/>
+      <c r="DR2" s="1"/>
+      <c r="DS2" s="1"/>
+      <c r="DT2" s="1"/>
+      <c r="DU2" s="1"/>
+      <c r="DV2" s="1"/>
+      <c r="DW2" s="1"/>
+      <c r="DX2" s="1"/>
+      <c r="DY2" s="1"/>
+      <c r="DZ2" s="1"/>
+      <c r="EA2" s="1"/>
+      <c r="EB2" s="1"/>
+      <c r="EC2" s="1"/>
+      <c r="ED2" s="1"/>
+      <c r="EE2" s="1"/>
+      <c r="EF2" s="1"/>
+      <c r="EG2" s="1"/>
+      <c r="EH2" s="1"/>
+      <c r="EI2" s="1"/>
+      <c r="EJ2" s="1"/>
+      <c r="EK2" s="1"/>
+      <c r="EL2" s="1"/>
+      <c r="EM2" s="1"/>
+      <c r="EN2" s="1"/>
+      <c r="EO2" s="1"/>
+      <c r="EP2" s="1"/>
+      <c r="EQ2" s="1"/>
+      <c r="ER2" s="1"/>
+      <c r="ES2" s="1"/>
+      <c r="ET2" s="1"/>
+      <c r="EU2" s="1"/>
+      <c r="EV2" s="1"/>
+      <c r="EW2" s="1"/>
+      <c r="EX2" s="1"/>
+      <c r="EY2" s="1"/>
+      <c r="EZ2" s="1"/>
+      <c r="FA2" s="1"/>
+      <c r="FB2" s="1"/>
+      <c r="FC2" s="1"/>
+      <c r="FD2" s="1"/>
+      <c r="FE2" s="1"/>
+      <c r="FF2" s="1"/>
+      <c r="FG2" s="1"/>
+      <c r="FH2" s="1"/>
+      <c r="FI2" s="1"/>
+      <c r="FJ2" s="1"/>
+      <c r="FK2" s="1"/>
+      <c r="FL2" s="1"/>
+      <c r="FM2" s="1"/>
+      <c r="FN2" s="1"/>
+      <c r="FO2" s="1"/>
+      <c r="FP2" s="1"/>
+      <c r="FQ2" s="1"/>
+      <c r="FR2" s="1"/>
+      <c r="FS2" s="1"/>
+      <c r="FT2" s="1"/>
+      <c r="FU2" s="1"/>
+      <c r="FV2" s="1"/>
+      <c r="FW2" s="1"/>
+      <c r="FX2" s="1"/>
+      <c r="FY2" s="1"/>
+      <c r="FZ2" s="1"/>
+      <c r="GA2" s="1"/>
+      <c r="GB2" s="1"/>
+      <c r="GC2" s="1"/>
+      <c r="GD2" s="1"/>
+      <c r="GE2" s="1"/>
+      <c r="GF2" s="1"/>
+      <c r="GG2" s="1"/>
+      <c r="GH2" s="1"/>
+      <c r="GI2" s="1"/>
+      <c r="GJ2" s="1"/>
+      <c r="GK2" s="1"/>
+      <c r="GL2" s="1"/>
+      <c r="GM2" s="1"/>
+      <c r="GN2" s="1"/>
+      <c r="GO2" s="1"/>
+      <c r="GP2" s="1"/>
+      <c r="GQ2" s="1"/>
+      <c r="GR2" s="1"/>
+      <c r="GS2" s="1"/>
+      <c r="GT2" s="1"/>
+      <c r="GU2" s="1"/>
+      <c r="GV2" s="1"/>
+      <c r="GW2" s="1"/>
+      <c r="GX2" s="1"/>
+      <c r="GY2" s="1"/>
+      <c r="GZ2" s="1"/>
+      <c r="HA2" s="1"/>
+      <c r="HB2" s="1"/>
+      <c r="HC2" s="1"/>
+      <c r="HD2" s="1"/>
+      <c r="HE2" s="1"/>
+      <c r="HF2" s="1"/>
+      <c r="HG2" s="1"/>
+      <c r="HH2" s="1"/>
+      <c r="HI2" s="1"/>
+      <c r="HJ2" s="1"/>
+      <c r="HK2" s="1"/>
+      <c r="HL2" s="1"/>
+      <c r="HM2" s="1"/>
+      <c r="HN2" s="1"/>
+      <c r="HO2" s="1"/>
+      <c r="HP2" s="1"/>
+      <c r="HQ2" s="1"/>
+      <c r="HR2" s="1"/>
+      <c r="HS2" s="1"/>
+      <c r="HT2" s="1"/>
+      <c r="HU2" s="1"/>
+      <c r="HV2" s="1"/>
+      <c r="HW2" s="1"/>
+      <c r="HX2" s="1"/>
+      <c r="HY2" s="1"/>
+      <c r="HZ2" s="1"/>
+      <c r="IA2" s="1"/>
+      <c r="IB2" s="1"/>
+      <c r="IC2" s="1"/>
+      <c r="ID2" s="1"/>
+      <c r="IE2" s="1"/>
+      <c r="IF2" s="1"/>
+      <c r="IG2" s="1"/>
+      <c r="IH2" s="1"/>
+      <c r="II2" s="1"/>
+      <c r="IJ2" s="1"/>
+      <c r="IK2" s="1"/>
+      <c r="IL2" s="1"/>
+      <c r="IM2" s="1"/>
+      <c r="IN2" s="1"/>
+      <c r="IO2" s="1"/>
+      <c r="IP2" s="1"/>
+      <c r="IQ2" s="1"/>
+      <c r="IR2" s="1"/>
+      <c r="IS2" s="1"/>
+      <c r="IT2" s="1"/>
+      <c r="IU2" s="1"/>
+      <c r="IV2" s="1"/>
+      <c r="IW2" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
[PHOENIX-6396] -ui updated users in login testdata sheet
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="19"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,688 +30,693 @@
     <sheet name="bifurcationDetails" sheetId="20" state="visible" r:id="rId21"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="226">
   <si>
-    <t>dataName</t>
-  </si>
-  <si>
-    <t>mobileNumber</t>
-  </si>
-  <si>
-    <t>ownerName</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>emailAddress</t>
-  </si>
-  <si>
-    <t>guardianRelation</t>
-  </si>
-  <si>
-    <t>guardian</t>
-  </si>
-  <si>
-    <t>bimal</t>
-  </si>
-  <si>
-    <t>Bimal</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>bimal@gmail.com</t>
-  </si>
-  <si>
-    <t>Father</t>
-  </si>
-  <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>reasonForCreation</t>
-  </si>
-  <si>
-    <t>extentOfSite</t>
-  </si>
-  <si>
-    <t>occupancyCertificateNumber</t>
-  </si>
-  <si>
-    <t>assessmentNewProperty</t>
-  </si>
-  <si>
-    <t>NEW PROPERTY</t>
-  </si>
-  <si>
-    <t>locality</t>
-  </si>
-  <si>
-    <t>zoneNumber</t>
-  </si>
-  <si>
-    <t>wardNumber</t>
-  </si>
-  <si>
-    <t>blockNumber</t>
-  </si>
-  <si>
-    <t>electionWard</t>
-  </si>
-  <si>
-    <t>doorNumber</t>
-  </si>
-  <si>
-    <t>pincode</t>
-  </si>
-  <si>
-    <t>addressOne</t>
-  </si>
-  <si>
-    <t>4th colony</t>
-  </si>
-  <si>
-    <t>Zone-1</t>
-  </si>
-  <si>
-    <t>Election Ward No. 1</t>
-  </si>
-  <si>
-    <t>12/46</t>
-  </si>
-  <si>
-    <t>lift</t>
-  </si>
-  <si>
-    <t>toilets</t>
-  </si>
-  <si>
-    <t>waterTap</t>
-  </si>
-  <si>
-    <t>electricity</t>
-  </si>
-  <si>
-    <t>attachedBathroom</t>
-  </si>
-  <si>
-    <t>waterHarvesting</t>
-  </si>
-  <si>
-    <t>cableConnection</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>floorType</t>
-  </si>
-  <si>
-    <t>roofType</t>
-  </si>
-  <si>
-    <t>wallType</t>
-  </si>
-  <si>
-    <t>woodType</t>
-  </si>
-  <si>
-    <t>defaultConstructionType</t>
-  </si>
-  <si>
-    <t>BAMBOO</t>
-  </si>
-  <si>
-    <t>Absheet</t>
-  </si>
-  <si>
-    <t>Allmixing</t>
-  </si>
-  <si>
-    <t>floorNumber</t>
-  </si>
-  <si>
-    <t>classificationOfBuilding</t>
-  </si>
-  <si>
-    <t>natureOfUsage</t>
-  </si>
-  <si>
-    <t>firmName</t>
-  </si>
-  <si>
-    <t>occupancy</t>
-  </si>
-  <si>
-    <t>occupantName</t>
-  </si>
-  <si>
-    <t>constructionDate</t>
-  </si>
-  <si>
-    <t>effectiveFromDate</t>
-  </si>
-  <si>
-    <t>unstructuredLand</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>breadth</t>
-  </si>
-  <si>
-    <t>buildingPermissionNumber</t>
-  </si>
-  <si>
-    <t>buildingPermissionDate</t>
-  </si>
-  <si>
-    <t>plinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t>firstFloor</t>
-  </si>
-  <si>
-    <t>1st floor</t>
-  </si>
-  <si>
-    <t>Huts</t>
-  </si>
-  <si>
-    <t>Residence</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>11/22</t>
-  </si>
-  <si>
-    <t>documentType</t>
-  </si>
-  <si>
-    <t>deedNo</t>
-  </si>
-  <si>
-    <t>deedDate</t>
-  </si>
-  <si>
-    <t>documentSelect</t>
-  </si>
-  <si>
-    <t>Registered Will Document</t>
-  </si>
-  <si>
-    <t>43051</t>
-  </si>
-  <si>
-    <t>20/12/2016</t>
-  </si>
-  <si>
-    <t>approverDepartment</t>
-  </si>
-  <si>
-    <t>approverDesignation</t>
-  </si>
-  <si>
-    <t>approver</t>
-  </si>
-  <si>
-    <t>approverRemarks</t>
-  </si>
-  <si>
-    <t>billCollector</t>
-  </si>
-  <si>
-    <t>REVENUE</t>
-  </si>
-  <si>
-    <t>Bill Collector</t>
-  </si>
-  <si>
-    <t>D.Khasim ~ REV_Bill Collector_1</t>
-  </si>
-  <si>
-    <t>Forward to bill collector</t>
-  </si>
-  <si>
-    <t>revenueInspector</t>
-  </si>
-  <si>
-    <t>UD Revenue Inspector</t>
-  </si>
-  <si>
-    <t>P.Sadiq Hussain ~ UD RI</t>
-  </si>
-  <si>
-    <t>Forward to revenue insoector</t>
-  </si>
-  <si>
-    <t>revenueOfficer</t>
-  </si>
-  <si>
-    <t>Revenue Officer</t>
-  </si>
-  <si>
-    <t>B.Veeraswamy ~ REV_Revenue Officer_3</t>
-  </si>
-  <si>
-    <t>Forward to revenue officer</t>
-  </si>
-  <si>
-    <t>commissioner</t>
-  </si>
-  <si>
-    <t>ADMINISTRATION</t>
-  </si>
-  <si>
-    <t>Commissioner</t>
-  </si>
-  <si>
-    <t>Ravindra Babu ~ ADM_Commissioner_2</t>
-  </si>
-  <si>
-    <t>Forward to commissioner</t>
-  </si>
-  <si>
-    <t>commissioner1</t>
-  </si>
-  <si>
-    <t>Ravindra Babu/ADM_Commissioner_2</t>
-  </si>
-  <si>
-    <t>engineer</t>
-  </si>
-  <si>
-    <t>ENGINEERING</t>
-  </si>
-  <si>
-    <t>Assistant Engineer</t>
-  </si>
-  <si>
-    <t>C.Naresh/ENG_Assistant Engineer_4</t>
-  </si>
-  <si>
-    <t>Forward to Engineer</t>
-  </si>
-  <si>
-    <t>engineer1</t>
-  </si>
-  <si>
-    <t>A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
-  </si>
-  <si>
-    <t>accountOfficer1</t>
-  </si>
-  <si>
-    <t>ACCOUNTS</t>
-  </si>
-  <si>
-    <t>Assistant Examiner of Accounts</t>
-  </si>
-  <si>
-    <t>Hanuman Prasad ~ ACC_AEOA_1</t>
-  </si>
-  <si>
-    <t>accountOfficer1a</t>
-  </si>
-  <si>
-    <t>K.Mohammed Juneed ~ ACC_AEOA_1</t>
-  </si>
-  <si>
-    <t>accountOfficer2</t>
-  </si>
-  <si>
-    <t>Examiner of Accounts</t>
-  </si>
-  <si>
-    <t>D Ramachandra Reddy ~ ACC_EOA_1</t>
-  </si>
-  <si>
-    <t>accountOfficer3</t>
-  </si>
-  <si>
-    <t>D Ramachandra Reddy/ACC_EOA_1</t>
-  </si>
-  <si>
-    <t>deputyExecutiveEngineer</t>
-  </si>
-  <si>
-    <t>Deputy Executive Engineer</t>
-  </si>
-  <si>
-    <t>S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
-  </si>
-  <si>
-    <t>sanitaryInspector</t>
-  </si>
-  <si>
-    <t>PUBLIC HEALTH AND SANITATION</t>
-  </si>
-  <si>
-    <t>Sanitary Inspector</t>
-  </si>
-  <si>
-    <t>Chandragiri Murali Krishna ~ PHS_Sanitary Inspector_1</t>
-  </si>
-  <si>
-    <t>Forward to Sanitary Inspector</t>
-  </si>
-  <si>
-    <t>propertyType</t>
-  </si>
-  <si>
-    <t>categoryOfOwnership</t>
-  </si>
-  <si>
-    <t>residentialPrivate</t>
-  </si>
-  <si>
-    <t>Residential</t>
-  </si>
-  <si>
-    <t>Private</t>
-  </si>
-  <si>
-    <t>assessmentAdditionProperty</t>
-  </si>
-  <si>
-    <t>editfloorNumber</t>
-  </si>
-  <si>
-    <t>editclassificationOfBuilding</t>
-  </si>
-  <si>
-    <t>editnatureOfUsage</t>
-  </si>
-  <si>
-    <t>editfirmName</t>
-  </si>
-  <si>
-    <t>editoccupancy</t>
-  </si>
-  <si>
-    <t>editoccupantName</t>
-  </si>
-  <si>
-    <t>editconstructionDate</t>
-  </si>
-  <si>
-    <t>editeffectiveFromDate</t>
-  </si>
-  <si>
-    <t>editunstructuredLand</t>
-  </si>
-  <si>
-    <t>editlength</t>
-  </si>
-  <si>
-    <t>editbreadth</t>
-  </si>
-  <si>
-    <t>editbuildingPermissionNumber</t>
-  </si>
-  <si>
-    <t>editbuildingPermissionDate</t>
-  </si>
-  <si>
-    <t>editplinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t>firstFloorAdditionaltaration</t>
-  </si>
-  <si>
-    <t>2nd Floor</t>
-  </si>
-  <si>
-    <t>Commercial</t>
-  </si>
-  <si>
-    <t>Sunil</t>
-  </si>
-  <si>
-    <t>33/22</t>
-  </si>
-  <si>
-    <t>fromDate</t>
-  </si>
-  <si>
-    <t>toDate</t>
-  </si>
-  <si>
-    <t>report1</t>
-  </si>
-  <si>
-    <t>06/12/2016</t>
-  </si>
-  <si>
-    <t>report2</t>
-  </si>
-  <si>
-    <t>07/12/2016</t>
-  </si>
-  <si>
-    <t>10/12/2016</t>
-  </si>
-  <si>
-    <t>message1</t>
-  </si>
-  <si>
-    <t>actualMessage</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>sellerExecutantName</t>
-  </si>
-  <si>
-    <t>buyerClaimantName</t>
-  </si>
-  <si>
-    <t>doorNo</t>
-  </si>
-  <si>
-    <t>propertyAddress</t>
-  </si>
-  <si>
-    <t>registeredPlotArea</t>
-  </si>
-  <si>
-    <t>registerPlinthArea</t>
-  </si>
-  <si>
-    <t>eastBoundary</t>
-  </si>
-  <si>
-    <t>westBoundary</t>
-  </si>
-  <si>
-    <t>northBoundary</t>
-  </si>
-  <si>
-    <t>southBoundary</t>
-  </si>
-  <si>
-    <t>sroName</t>
-  </si>
-  <si>
-    <t>reasonForChange</t>
-  </si>
-  <si>
-    <t>registrationDocumentNumber</t>
-  </si>
-  <si>
-    <t>registrationDocumentDate</t>
-  </si>
-  <si>
-    <t>partiesConsiderationValue</t>
-  </si>
-  <si>
-    <t>departmentGuide</t>
-  </si>
-  <si>
-    <t>register</t>
-  </si>
-  <si>
-    <t>Nadir</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Sro</t>
-  </si>
-  <si>
-    <t>Gift Deed</t>
-  </si>
-  <si>
-    <t>12/12/2016</t>
-  </si>
-  <si>
-    <t>dataRow</t>
-  </si>
-  <si>
-    <t>searchValue</t>
-  </si>
-  <si>
-    <t>searchValue2</t>
-  </si>
-  <si>
-    <t>searchWithAssessmentNumber</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>searchWithMobileNumber</t>
-  </si>
-  <si>
-    <t>0000161311</t>
-  </si>
-  <si>
-    <t>searchWithDoorNumber</t>
-  </si>
-  <si>
-    <t>87/1110-9-c</t>
-  </si>
-  <si>
-    <t>searchWithZoneAndWardNumber</t>
-  </si>
-  <si>
-    <t>Zone-15;Revenue Ward No  87</t>
-  </si>
-  <si>
-    <t>87/1110-9-c;C. Naga Sailaja W/o R. Satish Kumar</t>
-  </si>
-  <si>
-    <t>searchWithOwnerName</t>
-  </si>
-  <si>
-    <t>revenue colony;C. Naga Sailaja W/o R. Satish Kumar</t>
-  </si>
-  <si>
-    <t>searchByDemand</t>
-  </si>
-  <si>
-    <t>500;501</t>
-  </si>
-  <si>
-    <t>revisionPetitionDetails</t>
-  </si>
-  <si>
-    <t>revisionpetitionBlock</t>
-  </si>
-  <si>
-    <t>Revision Started</t>
-  </si>
-  <si>
-    <t>hearingDate</t>
-  </si>
-  <si>
-    <t>hearingTime</t>
-  </si>
-  <si>
-    <t>venue</t>
-  </si>
-  <si>
-    <t>hearingBlock</t>
-  </si>
-  <si>
-    <t>28/06/2017</t>
-  </si>
-  <si>
-    <t>9.30 AM</t>
-  </si>
-  <si>
-    <t>reasonForDemolition</t>
-  </si>
-  <si>
-    <t>surveyNumber</t>
-  </si>
-  <si>
-    <t>pattaNumber</t>
-  </si>
-  <si>
-    <t>marketValue</t>
-  </si>
-  <si>
-    <t>capitalValue</t>
-  </si>
-  <si>
-    <t>North</t>
-  </si>
-  <si>
-    <t>East</t>
-  </si>
-  <si>
-    <t>West</t>
-  </si>
-  <si>
-    <t>South</t>
-  </si>
-  <si>
-    <t>demolitionBlock</t>
-  </si>
-  <si>
-    <t>Demolition of property</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>pqr</t>
-  </si>
-  <si>
-    <t>lmn</t>
-  </si>
-  <si>
-    <t>parentAssessmentNo</t>
-  </si>
-  <si>
-    <t>bifurcationProperty</t>
-  </si>
-  <si>
-    <t>BIFURCATION</t>
+    <t xml:space="preserve">dataName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ownerName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emailAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guardianRelation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guardian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bimal@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonForCreation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extentOfSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupancyCertificateNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentNewProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW PROPERTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zoneNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wardNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blockNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electionWard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pincode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressOne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4th colony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Election Ward No. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toilets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterTap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attachedBathroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterHarvesting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cableConnection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">floorType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roofType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wallType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">woodType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">defaultConstructionType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAMBOO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allmixing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">floorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">classificationOfBuilding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natureOfUsage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firmName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constructionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effectiveFromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unstructuredLand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">breadth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buildingPermissionNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buildingPermissionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstFloor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deedNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deedDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentSelect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registered Will Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approverDepartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approverDesignation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approverRemarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billCollector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REVENUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bill Collector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D.Khasim ~ REV_Bill Collector_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to bill collector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenueInspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UD Revenue Inspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.N.N.Rajeswara Rao ~ UD_Revenue Inspector_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to revenue insoector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenueOfficer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue Officer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.Veeraswamy ~ REV_Revenue Officer_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to revenue officer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commissioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADMINISTRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commissioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ravindra Babu ~ ADM_Commissioner_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to commissioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commissioner1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ravindra Babu/ADM_Commissioner_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENGINEERING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.Naresh/ENG_Assistant Engineer_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engineer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCOUNTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant Examiner of Accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hanuman Prasad ~ ACC_AEOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K.Mohammed Juneed ~ ACC_AEOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examiner of Accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D Ramachandra Reddy ~ ACC_EOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D Ramachandra Reddy/ACC_EOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deputyExecutiveEngineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deputy Executive Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sanitaryInspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUBLIC HEALTH AND SANITATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanitary Inspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chandragiri Murali Krishna ~ PHS_Sanitary Inspector_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to Sanitary Inspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">propertyType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categoryOfOwnership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residentialPrivate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Private</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentAdditionProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editfloorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editclassificationOfBuilding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editnatureOfUsage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editfirmName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editoccupancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editoccupantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editconstructionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editeffectiveFromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editunstructuredLand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editlength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbreadth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbuildingPermissionNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbuildingPermissionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editplinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstFloorAdditionaltaration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd Floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commercial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actualMessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sellerExecutantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buyerClaimantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doorNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">propertyAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registeredPlotArea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registerPlinthArea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eastBoundary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">westBoundary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">northBoundary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">southBoundary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sroName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonForChange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registrationDocumentNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registrationDocumentDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partiesConsiderationValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">departmentGuide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nadir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangalore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gift Deed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataRow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchValue2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchWithAssessmentNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchWithMobileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000161311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchWithDoorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87/1110-9-c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchWithZoneAndWardNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone-15;Revenue Ward No  87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87/1110-9-c;C. Naga Sailaja W/o R. Satish Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchWithOwnerName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenue colony;C. Naga Sailaja W/o R. Satish Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchByDemand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500;501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revisionPetitionDetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revisionpetitionBlock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revision Started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hearingDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hearingTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hearingBlock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/06/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.30 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonForDemolition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surveyNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pattaNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marketValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capitalValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demolitionBlock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demolition of property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xyz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pqr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lmn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parentAssessmentNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bifurcationProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIFURCATION</t>
   </si>
 </sst>
 </file>
@@ -719,7 +724,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
@@ -944,13 +949,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,11 +1031,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.6275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.4081632653061"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.4132653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1080,15 +1085,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.484693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1209,11 +1214,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,11 +1267,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.44897959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1315,10 +1319,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1362,25 +1366,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1514,10 +1518,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="40.765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.6632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,9 +1621,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1662,11 +1666,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,9 +1724,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1812,13 +1813,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="48.3265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="37.6632653061224"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,19 +1870,18 @@
   </sheetPr>
   <dimension ref="A1:IW2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.7857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.5663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2444,14 +2444,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2524,8 +2524,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2611,9 +2611,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40.5"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2676,25 +2676,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="40.5"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="43.6020408163265"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="37.6632653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2815,11 +2815,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2868,19 +2868,19 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="43.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="67.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="44.4132653061225"/>
-    <col collapsed="false" hidden="false" max="257" min="6" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="42.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="66.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="257" min="6" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3151,11 +3151,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-6396] -ui updated excel reader of property tax
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,8 +15,8 @@
     <sheet name="constructionTypeDetails" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="floorDetails" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="documentDetails" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="propertyHeaderDetails" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="editAssessmentDetails" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="editAssessmentDetails" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="propertyHeaderDetails" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="editFloorDetails" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="vltReport" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="ptReport" sheetId="12" state="visible" r:id="rId13"/>
@@ -265,6 +265,9 @@
     <t xml:space="preserve">20/12/2016</t>
   </si>
   <si>
+    <t xml:space="preserve">assessmentAdditionProperty</t>
+  </si>
+  <si>
     <t xml:space="preserve">propertyType</t>
   </si>
   <si>
@@ -278,9 +281,6 @@
   </si>
   <si>
     <t xml:space="preserve">Private</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentAdditionProperty</t>
   </si>
   <si>
     <t xml:space="preserve">editfloorNumber</t>
@@ -784,13 +784,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,15 +865,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.484693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,11 +994,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.44897959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1048,10 +1046,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1100,10 +1099,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1147,25 +1146,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1299,10 +1297,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="39.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.8520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="38.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.9081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1402,9 +1400,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1447,11 +1445,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1505,6 +1503,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1588,18 +1589,19 @@
   </sheetPr>
   <dimension ref="A1:IW2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,10 +1880,10 @@
         <v>175</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1016094473</v>
+        <v>1016094460</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>111</v>
@@ -2162,13 +2164,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="37.6632653061224"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,14 +2226,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,8 +2305,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2392,9 +2391,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.6071428571429"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2457,25 +2455,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="43.6020408163265"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="37.6632653061224"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="42.5204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="38.6071428571429"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2596,11 +2593,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2647,88 +2644,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>75</v>
+      <c r="B1" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.4132653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.3265306122449"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>5000</v>
@@ -2747,4 +2691,56 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.77551020408163"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[PHOENIX-6817] Added one negetive test case
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -784,12 +784,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -844,7 +845,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -865,15 +866,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49.2704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,7 +973,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -994,10 +994,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,7 +1026,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1046,11 +1047,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1078,7 +1079,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1099,10 +1100,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1125,7 +1125,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1146,24 +1146,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1276,7 +1277,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1297,10 +1298,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="38.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.9081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1379,7 +1380,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1400,9 +1401,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1424,7 +1425,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1445,11 +1446,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1483,7 +1484,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1504,7 +1505,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1574,7 +1575,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1589,19 +1590,19 @@
   </sheetPr>
   <dimension ref="A1:IW2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,7 +2144,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2164,12 +2165,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="36.8520408163265"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2205,7 +2207,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2220,19 +2222,20 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2284,7 +2287,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2305,7 +2308,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2370,7 +2374,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2391,8 +2395,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2434,7 +2439,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2455,24 +2460,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="36.8520408163265"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,7 +2578,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2593,11 +2599,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2631,7 +2637,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2652,11 +2658,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.3316326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2685,7 +2690,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2706,10 +2711,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2737,7 +2743,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[PHOENIX-5847] Modified the PTIS module test cases
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -784,13 +784,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,14 +865,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.515306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="46.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,11 +994,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,11 +1046,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1100,9 +1099,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1146,25 +1146,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1298,10 +1297,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,9 +1400,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1446,11 +1445,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1505,7 +1504,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1596,13 +1595,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2165,13 +2164,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2222,20 +2220,19 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,8 +2305,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2395,9 +2391,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2454,31 +2449,29 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O14" activeCellId="0" sqref="O14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="41.0357142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="40.5"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2551,10 +2544,10 @@
         <v>8</v>
       </c>
       <c r="H2" s="5" t="n">
-        <v>42653</v>
+        <v>42835</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>42654</v>
+        <v>42866</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>66</v>
@@ -2599,11 +2592,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2658,10 +2651,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2705,17 +2699,16 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-6817]-Ui updated email address of property tax
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -778,18 +778,19 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,12 +816,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>2299087661</v>
+        <v>2222223451</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -844,7 +845,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -865,15 +866,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="46.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.8979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,7 +974,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -994,10 +995,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,7 +1027,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1046,11 +1048,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1078,7 +1079,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1099,10 +1100,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1125,7 +1126,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1146,24 +1147,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1276,7 +1278,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1297,10 +1299,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1379,7 +1381,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1400,9 +1402,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1424,7 +1426,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1445,11 +1447,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1483,7 +1485,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1503,9 +1505,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1574,7 +1573,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1595,13 +1594,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9795918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,7 +2141,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2158,18 +2156,19 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.7397959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2205,7 +2204,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2226,13 +2225,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2284,7 +2284,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2300,12 +2300,13 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2370,7 +2371,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2391,8 +2392,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2434,7 +2436,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2449,29 +2451,31 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="40.5"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2571,7 +2575,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2592,11 +2596,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2630,7 +2634,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2651,11 +2655,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="44.8163265306122"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2684,7 +2688,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2705,10 +2709,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2736,7 +2741,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[PHOENIX-5879] UI : Modified the data for DataEntryScreen in PTIS
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="177">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -118,10 +118,10 @@
     <t xml:space="preserve">addressOne</t>
   </si>
   <si>
-    <t xml:space="preserve">4th colony</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone-1</t>
+    <t xml:space="preserve">abass nagar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone1</t>
   </si>
   <si>
     <t xml:space="preserve">Election Ward No. 1</t>
@@ -226,109 +226,112 @@
     <t xml:space="preserve">1st floor</t>
   </si>
   <si>
+    <t xml:space="preserve">HUTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deedNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deedDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentSelect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registered Will Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentAdditionProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">propertyType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categoryOfOwnership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residentialPrivate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Private</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editfloorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editclassificationOfBuilding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editnatureOfUsage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editfirmName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editoccupancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editoccupantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editconstructionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editeffectiveFromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editunstructuredLand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editlength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbreadth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbuildingPermissionNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbuildingPermissionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editplinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstFloorAdditionaltaration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd Floor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Huts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deedNo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deedDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentSelect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registered Will Document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentAdditionProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">propertyType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categoryOfOwnership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">residentialPrivate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Private</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editfloorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editclassificationOfBuilding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editnatureOfUsage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editfirmName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editoccupancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editoccupantName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editconstructionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editeffectiveFromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editunstructuredLand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editlength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbreadth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbuildingPermissionNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbuildingPermissionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editplinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstFloorAdditionaltaration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd Floor</t>
   </si>
   <si>
     <t xml:space="preserve">Commercial</t>
@@ -778,19 +781,19 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,15 +869,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.8979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,7 +934,7 @@
         <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>63</v>
@@ -941,10 +943,10 @@
         <v>64</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>42319</v>
@@ -962,7 +964,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N2" s="5" t="n">
         <v>42358</v>
@@ -995,11 +997,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,21 +1009,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1048,10 +1050,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1059,21 +1062,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1100,10 +1103,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1111,15 +1113,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1147,25 +1149,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,69 +1175,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>30</v>
@@ -1244,28 +1246,28 @@
         <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N2" s="6" t="n">
         <v>121</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="P2" s="6" t="n">
         <v>500000</v>
@@ -1299,81 +1301,81 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B2" s="15" t="n">
         <v>1016063818</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1402,25 +1404,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1447,39 +1449,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1505,45 +1507,48 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>111</v>
@@ -1558,16 +1563,16 @@
         <v>300</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1594,12 +1599,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,7 +1616,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
@@ -1872,10 +1878,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1016094460</v>
@@ -2162,13 +2168,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.25"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.75"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2219,20 +2225,20 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.9438775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,8 +2311,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2392,9 +2398,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,31 +2457,31 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="33.75"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2596,11 +2602,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2655,11 +2661,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="43.7397959183673"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="43.1989795918367"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,11 +2714,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5848]-ui updated excel data of create new property
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">abass nagar</t>
   </si>
   <si>
-    <t xml:space="preserve">Zone1</t>
+    <t xml:space="preserve">Zone-11</t>
   </si>
   <si>
     <t xml:space="preserve">Election Ward No. 1</t>
@@ -226,7 +226,7 @@
     <t xml:space="preserve">1st floor</t>
   </si>
   <si>
-    <t xml:space="preserve">HUTS</t>
+    <t xml:space="preserve">cements</t>
   </si>
   <si>
     <t xml:space="preserve">Residence</t>
@@ -782,18 +782,17 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,7 +823,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>2222223451</v>
+        <v>2222223444</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -869,14 +868,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -997,11 +997,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,11 +1049,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1103,9 +1102,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1149,25 +1149,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,10 +1300,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1404,9 +1403,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1449,11 +1448,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,7 +1507,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1599,13 +1598,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2168,13 +2167,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.25"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.75"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.7142857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,20 +2223,19 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.9438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,8 +2308,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2398,9 +2394,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2457,31 +2452,29 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="39.1479591836735"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="33.75"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="38.6071428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2602,11 +2595,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2661,10 +2654,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="43.1989795918367"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2714,11 +2708,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-6113] UI : Fixed Create Data Entry Screen Automation for PropertyTax
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="179">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">abass nagar</t>
   </si>
   <si>
-    <t xml:space="preserve">Zone-11</t>
+    <t xml:space="preserve">Zone1</t>
   </si>
   <si>
     <t xml:space="preserve">Election Ward No. 1</t>
@@ -229,109 +229,115 @@
     <t xml:space="preserve">cements</t>
   </si>
   <si>
+    <t xml:space="preserve">Residencial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirmName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deedNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deedDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentSelect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registered Will Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentAdditionProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">propertyType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categoryOfOwnership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residentialPrivate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Private</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editfloorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editclassificationOfBuilding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editnatureOfUsage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editfirmName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editoccupancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editoccupantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editconstructionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editeffectiveFromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editunstructuredLand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editlength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbreadth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbuildingPermissionNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbuildingPermissionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editplinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstFloorAdditionaltaration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd Floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huts</t>
+  </si>
+  <si>
     <t xml:space="preserve">Residence</t>
   </si>
   <si>
     <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deedNo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deedDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentSelect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registered Will Document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentAdditionProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">propertyType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categoryOfOwnership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">residentialPrivate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Private</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editfloorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editclassificationOfBuilding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editnatureOfUsage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editfirmName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editoccupancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editoccupantName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editconstructionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editeffectiveFromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editunstructuredLand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editlength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbreadth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbuildingPermissionNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbuildingPermissionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editplinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstFloorAdditionaltaration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd Floor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huts</t>
   </si>
   <si>
     <t xml:space="preserve">Commercial</t>
@@ -787,12 +793,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -868,15 +875,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,16 +944,16 @@
         <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>42319</v>
@@ -964,7 +971,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="N2" s="5" t="n">
         <v>42358</v>
@@ -997,10 +1004,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1008,21 +1016,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1049,11 +1057,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1061,21 +1069,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1102,10 +1110,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1113,15 +1121,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1149,24 +1157,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3112244897959"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.5204081632653"/>
     <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,69 +1183,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>30</v>
@@ -1245,28 +1254,28 @@
         <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="N2" s="6" t="n">
         <v>121</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="P2" s="6" t="n">
         <v>500000</v>
@@ -1300,81 +1309,80 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9948979591837"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B2" s="15" t="n">
         <v>1016063818</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>140</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1403,25 +1411,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1448,39 +1455,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1507,47 +1513,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>111</v>
@@ -1562,16 +1568,16 @@
         <v>300</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1598,13 +1604,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1615,7 +1621,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
@@ -1877,10 +1883,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1016094460</v>
@@ -2167,12 +2173,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.7142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,19 +2230,20 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,7 +2316,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2394,8 +2403,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.8265306122449"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2452,29 +2462,32 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="34.8265306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2595,11 +2608,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2654,11 +2666,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="42.25"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2708,10 +2720,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5847] UI : Working On PropertyTax Automation
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -331,7 +331,7 @@
     <t xml:space="preserve">2nd Floor</t>
   </si>
   <si>
-    <t xml:space="preserve">Huts</t>
+    <t xml:space="preserve">HUTSSS</t>
   </si>
   <si>
     <t xml:space="preserve">Residence</t>
@@ -793,13 +793,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,21 +869,21 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.6020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,11 +1004,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1057,11 +1057,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1110,10 +1109,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1157,25 +1156,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.0408163265306"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.25"/>
     <col collapsed="false" hidden="false" max="257" min="18" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1309,9 +1308,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1411,8 +1411,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1455,10 +1456,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1512,9 +1514,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1604,13 +1603,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2173,13 +2171,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2236,14 +2234,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2316,8 +2314,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2403,9 +2401,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,32 +2460,32 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.8673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2608,10 +2606,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2666,11 +2665,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.8775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="42.25"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.3367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="41.7142857142857"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2720,11 +2719,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>